<commit_message>
form for staff added
</commit_message>
<xml_diff>
--- a/public/files/filename.xlsx
+++ b/public/files/filename.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
-  <si>
-    <t>REGNO</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+  <si>
+    <t>REG.NO.</t>
   </si>
   <si>
     <t>NAME</t>
@@ -47,12 +47,18 @@
     <t>SEM1[PH6151]</t>
   </si>
   <si>
+    <t>BATCH</t>
+  </si>
+  <si>
     <t>ABINAYA S</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
+    <t xml:space="preserve">2015 - 2018 </t>
+  </si>
+  <si>
     <t>ABISHEK M V</t>
   </si>
   <si>
@@ -75,6 +81,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>2015 - 2018</t>
   </si>
   <si>
     <t>AKILAN A</t>
@@ -1414,7 +1423,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1431,7 +1440,8 @@
     <col min="9" max="9" width="16.3516" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.3516" style="1" customWidth="1"/>
-    <col min="12" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.3516" style="1" customWidth="1"/>
+    <col min="13" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.7" customHeight="1">
@@ -1465,8 +1475,11 @@
       <c r="J1" t="s" s="3">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="4">
+      <c r="K1" t="s" s="3">
         <v>10</v>
+      </c>
+      <c r="L1" t="s" s="4">
+        <v>11</v>
       </c>
     </row>
     <row r="2" ht="20.7" customHeight="1">
@@ -1474,34 +1487,37 @@
         <v>910714104001</v>
       </c>
       <c r="B2" t="s" s="6">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K2" t="s" s="3">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="L2" t="s" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="3" ht="20.7" customHeight="1">
@@ -1509,34 +1525,37 @@
         <v>910714104002</v>
       </c>
       <c r="B3" t="s" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s" s="3">
         <v>14</v>
-      </c>
-      <c r="D3" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s" s="3">
-        <v>18</v>
       </c>
     </row>
     <row r="4" ht="20.7" customHeight="1">
@@ -1544,34 +1563,37 @@
         <v>910714104003</v>
       </c>
       <c r="B4" t="s" s="6">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L4" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="5" ht="20.7" customHeight="1">
@@ -1579,33 +1601,36 @@
         <v>910714104004</v>
       </c>
       <c r="B5" t="s" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K5" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="L5" t="s" s="3">
         <v>14</v>
       </c>
     </row>
@@ -1614,34 +1639,37 @@
         <v>910714104005</v>
       </c>
       <c r="B6" t="s" s="6">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L6" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="7" ht="20.7" customHeight="1">
@@ -1649,34 +1677,37 @@
         <v>910714104006</v>
       </c>
       <c r="B7" t="s" s="6">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G7" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I7" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K7" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="L7" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="8" ht="20.7" customHeight="1">
@@ -1684,34 +1715,37 @@
         <v>910714104007</v>
       </c>
       <c r="B8" t="s" s="6">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L8" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="20.7" customHeight="1">
@@ -1719,34 +1753,37 @@
         <v>910714104008</v>
       </c>
       <c r="B9" t="s" s="6">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="L9" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="26.7" customHeight="1">
@@ -1754,34 +1791,37 @@
         <v>910714104009</v>
       </c>
       <c r="B10" t="s" s="6">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G10" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K10" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L10" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="11" ht="20.7" customHeight="1">
@@ -1789,34 +1829,37 @@
         <v>910714104010</v>
       </c>
       <c r="B11" t="s" s="6">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="L11" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="12" ht="20.7" customHeight="1">
@@ -1824,34 +1867,37 @@
         <v>910714104011</v>
       </c>
       <c r="B12" t="s" s="6">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F12" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I12" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K12" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L12" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="13" ht="20.7" customHeight="1">
@@ -1859,34 +1905,37 @@
         <v>910714104012</v>
       </c>
       <c r="B13" t="s" s="6">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K13" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L13" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="14" ht="26.7" customHeight="1">
@@ -1894,34 +1943,37 @@
         <v>910714104013</v>
       </c>
       <c r="B14" t="s" s="6">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H14" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I14" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J14" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K14" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="L14" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="15" ht="20.7" customHeight="1">
@@ -1929,34 +1981,37 @@
         <v>910714104014</v>
       </c>
       <c r="B15" t="s" s="6">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D15" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E15" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F15" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G15" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I15" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J15" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K15" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="L15" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="16" ht="20.7" customHeight="1">
@@ -1964,34 +2019,37 @@
         <v>910714104015</v>
       </c>
       <c r="B16" t="s" s="6">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E16" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F16" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G16" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H16" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J16" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K16" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="L16" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="17" ht="20.7" customHeight="1">
@@ -1999,34 +2057,37 @@
         <v>910714104016</v>
       </c>
       <c r="B17" t="s" s="6">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I17" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J17" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K17" t="s" s="3">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="L17" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="18" ht="20.7" customHeight="1">
@@ -2034,34 +2095,37 @@
         <v>910714104017</v>
       </c>
       <c r="B18" t="s" s="6">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H18" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I18" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J18" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K18" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L18" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="19" ht="20.7" customHeight="1">
@@ -2069,34 +2133,37 @@
         <v>910714104018</v>
       </c>
       <c r="B19" t="s" s="6">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G19" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K19" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L19" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="20" ht="20.7" customHeight="1">
@@ -2104,34 +2171,37 @@
         <v>910714104019</v>
       </c>
       <c r="B20" t="s" s="6">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D20" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H20" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I20" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J20" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K20" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L20" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="20.7" customHeight="1">
@@ -2139,34 +2209,37 @@
         <v>910714104020</v>
       </c>
       <c r="B21" t="s" s="6">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D21" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="H21" t="s" s="3">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="K21" t="s" s="3">
+        <v>17</v>
+      </c>
+      <c r="L21" t="s" s="3">
         <v>14</v>
-      </c>
-      <c r="F21" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="G21" t="s" s="3">
-        <v>16</v>
-      </c>
-      <c r="H21" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="I21" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="J21" t="s" s="3">
-        <v>14</v>
-      </c>
-      <c r="K21" t="s" s="3">
-        <v>15</v>
       </c>
     </row>
     <row r="22" ht="20.7" customHeight="1">
@@ -2174,34 +2247,37 @@
         <v>910714104021</v>
       </c>
       <c r="B22" t="s" s="6">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G22" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H22" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I22" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J22" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K22" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L22" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="23" ht="20.7" customHeight="1">
@@ -2209,34 +2285,37 @@
         <v>910714104022</v>
       </c>
       <c r="B23" t="s" s="6">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G23" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H23" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I23" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J23" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K23" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L23" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="24" ht="20.7" customHeight="1">
@@ -2244,34 +2323,37 @@
         <v>910714104023</v>
       </c>
       <c r="B24" t="s" s="6">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E24" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H24" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I24" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J24" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K24" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L24" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="25" ht="26.7" customHeight="1">
@@ -2279,34 +2361,37 @@
         <v>910714104024</v>
       </c>
       <c r="B25" t="s" s="6">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F25" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G25" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H25" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I25" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J25" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K25" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L25" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="26" ht="20.7" customHeight="1">
@@ -2314,34 +2399,37 @@
         <v>910714104026</v>
       </c>
       <c r="B26" t="s" s="6">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D26" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E26" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F26" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G26" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H26" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I26" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J26" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K26" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L26" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="27" ht="20.7" customHeight="1">
@@ -2349,33 +2437,36 @@
         <v>910714104027</v>
       </c>
       <c r="B27" t="s" s="6">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E27" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G27" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H27" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I27" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J27" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K27" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="L27" t="s" s="3">
         <v>14</v>
       </c>
     </row>
@@ -2384,33 +2475,36 @@
         <v>910714104028</v>
       </c>
       <c r="B28" t="s" s="6">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E28" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G28" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H28" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I28" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J28" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K28" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="L28" t="s" s="3">
         <v>14</v>
       </c>
     </row>
@@ -2419,34 +2513,37 @@
         <v>910714104029</v>
       </c>
       <c r="B29" t="s" s="6">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E29" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G29" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H29" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I29" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J29" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K29" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L29" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="30" ht="26.7" customHeight="1">
@@ -2454,33 +2551,36 @@
         <v>910714104030</v>
       </c>
       <c r="B30" t="s" s="6">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E30" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G30" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H30" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I30" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J30" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K30" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="L30" t="s" s="3">
         <v>14</v>
       </c>
     </row>
@@ -2489,34 +2589,37 @@
         <v>910714104031</v>
       </c>
       <c r="B31" t="s" s="6">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G31" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H31" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I31" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J31" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K31" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L31" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="32" ht="20.7" customHeight="1">
@@ -2524,34 +2627,37 @@
         <v>910714104032</v>
       </c>
       <c r="B32" t="s" s="6">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D32" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G32" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I32" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J32" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K32" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L32" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="33" ht="26.7" customHeight="1">
@@ -2559,34 +2665,37 @@
         <v>910714104033</v>
       </c>
       <c r="B33" t="s" s="6">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H33" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K33" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L33" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="34" ht="20.7" customHeight="1">
@@ -2594,34 +2703,37 @@
         <v>910714104034</v>
       </c>
       <c r="B34" t="s" s="6">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D34" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F34" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G34" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H34" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I34" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J34" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K34" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L34" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="35" ht="20.7" customHeight="1">
@@ -2629,34 +2741,37 @@
         <v>910714104035</v>
       </c>
       <c r="B35" t="s" s="6">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E35" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F35" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G35" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H35" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I35" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J35" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K35" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="L35" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="36" ht="20.7" customHeight="1">
@@ -2664,34 +2779,37 @@
         <v>910714104036</v>
       </c>
       <c r="B36" t="s" s="6">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F36" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G36" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H36" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I36" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J36" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K36" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L36" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="37" ht="20.7" customHeight="1">
@@ -2699,34 +2817,37 @@
         <v>910714104037</v>
       </c>
       <c r="B37" t="s" s="6">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E37" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F37" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G37" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H37" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I37" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J37" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K37" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L37" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="38" ht="20.7" customHeight="1">
@@ -2734,34 +2855,37 @@
         <v>910714104038</v>
       </c>
       <c r="B38" t="s" s="6">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D38" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E38" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F38" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G38" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H38" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I38" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J38" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K38" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L38" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="39" ht="26.7" customHeight="1">
@@ -2769,34 +2893,37 @@
         <v>910714104039</v>
       </c>
       <c r="B39" t="s" s="6">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E39" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F39" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G39" t="s" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H39" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I39" t="s" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="J39" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K39" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="L39" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
     <row r="40" ht="20.7" customHeight="1">
@@ -2804,34 +2931,37 @@
         <v>910714104040</v>
       </c>
       <c r="B40" t="s" s="8">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E40" t="s" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F40" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G40" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H40" t="s" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I40" t="s" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J40" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K40" t="s" s="3">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="L40" t="s" s="3">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2840,7 +2970,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:K40">
+  <conditionalFormatting sqref="C3:L40">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal" stopIfTrue="1">
       <formula>"u"</formula>
     </cfRule>

</xml_diff>